<commit_message>
Updated Acceptance testing cheet
</commit_message>
<xml_diff>
--- a/Acceptance test.xlsx
+++ b/Acceptance test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Documents/Concordia/Winter2018/SOEN341/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SebastienD/Desktop/Soen341/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDB44A66-89CD-2A46-9C98-39390B7B89FE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB857DC-A76A-CE42-AA2F-276C2A3DF145}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14680" xr2:uid="{153C621A-1283-484D-8D12-0A54F2A8130A}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="14600" xr2:uid="{153C621A-1283-484D-8D12-0A54F2A8130A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>User can create an account (sign up)</t>
   </si>
@@ -87,18 +87,12 @@
     <t>Users can see all questions posted by all users</t>
   </si>
   <si>
-    <t>Answers are rejected if they have more than 3 votes and more than 60 % downvotes</t>
-  </si>
-  <si>
     <t>User can delete answer</t>
   </si>
   <si>
     <t>Answers are listed after their questions</t>
   </si>
   <si>
-    <t>Answers are sorted by their votes</t>
-  </si>
-  <si>
     <t>Answers</t>
   </si>
   <si>
@@ -121,6 +115,27 @@
   </si>
   <si>
     <t>User panel</t>
+  </si>
+  <si>
+    <t>Users can upvote all questions</t>
+  </si>
+  <si>
+    <t>Users can downvote all questions</t>
+  </si>
+  <si>
+    <t>User can only have one active vote per question</t>
+  </si>
+  <si>
+    <t>Questions are rejected if they have more than 10 votes and more than 60 % downvotes</t>
+  </si>
+  <si>
+    <t>Answers are rejected if they have more than 10 votes and more than 60 % downvotes</t>
+  </si>
+  <si>
+    <t>Questions are sorted by their score</t>
+  </si>
+  <si>
+    <t>Answers are sorted by their score</t>
   </si>
 </sst>
 </file>
@@ -152,7 +167,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -274,11 +289,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -291,9 +317,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,15 +637,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A9CA3A-2E4C-F341-A85F-01CA02BB375C}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="108" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.5" customWidth="1"/>
+    <col min="1" max="1" width="72" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -736,64 +765,64 @@
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
+      <c r="A17" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>21</v>
+      <c r="A18" s="16" t="s">
+        <v>32</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>25</v>
+      <c r="A19" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="A20" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -801,7 +830,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -809,7 +838,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -817,51 +846,86 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>17</v>
+      <c r="A26" t="s">
+        <v>25</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
-        <v>30</v>
+      <c r="A29" t="s">
+        <v>21</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>